<commit_message>
modified dialog to have text process and delay next
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAEB14A-15B8-49C7-BE06-92CB62DC8F1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9182BB6-2A27-49F9-BD54-DAA061E66710}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="1890" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Key</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>Mr. Pengu and the Unlikely Denominators</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Test 123 123</t>
   </si>
 </sst>
 </file>
@@ -376,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,9 +426,17 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
victory stuff, game flow
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9182BB6-2A27-49F9-BD54-DAA061E66710}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9941B39-16FA-4098-BDBC-60F09B668524}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="1890" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Key</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Test 123 123</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,6 +446,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
more number ops art/animation, card deck art
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49131B50-D014-4195-A77B-6BEA9A097CDA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30E3EA2-B501-4282-AC15-60CB1C5CE3BE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="1890" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Key</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>CLOSE</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>SUBMIT</t>
   </si>
 </sst>
 </file>
@@ -430,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,9 +552,17 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update levels with ui, added 'ready'
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30E3EA2-B501-4282-AC15-60CB1C5CE3BE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAFD3F8-11AC-4102-A76C-E65B07B3826D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="1890" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Key</t>
   </si>
@@ -43,9 +43,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>Mr. Pengu and the Unlikely Denominators</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -104,6 +101,21 @@
   </si>
   <si>
     <t>SUBMIT</t>
+  </si>
+  <si>
+    <t>ATTACK</t>
+  </si>
+  <si>
+    <t>DEFEND</t>
+  </si>
+  <si>
+    <t>Pengu and the Unlikely Encounters</t>
+  </si>
+  <si>
+    <t>attack</t>
+  </si>
+  <si>
+    <t>defend</t>
   </si>
 </sst>
 </file>
@@ -436,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,10 +492,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -491,79 +503,95 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
         <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more debug stuff for gameplay, victory ui art/animation
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAFD3F8-11AC-4102-A76C-E65B07B3826D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7978DD1F-7E62-4C38-AF07-60AB6DF7080B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="1890" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30945" yWindow="1590" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Key</t>
   </si>
@@ -116,6 +116,30 @@
   </si>
   <si>
     <t>defend</t>
+  </si>
+  <si>
+    <t>rounds</t>
+  </si>
+  <si>
+    <t>ROUNDS</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>revivePenalty</t>
+  </si>
+  <si>
+    <t>REVIVE PENALTY</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -448,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,6 +618,38 @@
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
more level 1 animations, dialog, instruct
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7978DD1F-7E62-4C38-AF07-60AB6DF7080B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2A0586-DF60-433D-8119-5CAD8221B57D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30945" yWindow="1590" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="1635" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Key</t>
   </si>
@@ -140,6 +140,66 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>level_1_intro_1</t>
+  </si>
+  <si>
+    <t>A chasm impedes Pengu's journey.</t>
+  </si>
+  <si>
+    <t>level_1_intro_2</t>
+  </si>
+  <si>
+    <t>Help Pengu out by determining the distance of the gap!</t>
+  </si>
+  <si>
+    <t>level_1_info_1</t>
+  </si>
+  <si>
+    <t>level_1_info_3</t>
+  </si>
+  <si>
+    <t>level_1_info_4</t>
+  </si>
+  <si>
+    <t>level_1_info_5</t>
+  </si>
+  <si>
+    <t>level_1_info_2_a</t>
+  </si>
+  <si>
+    <t>level_1_info_2_b</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>SUCCESS!</t>
+  </si>
+  <si>
+    <t>In order to add these two fractions, you must make the denominators equal.</t>
+  </si>
+  <si>
+    <t>One way to do this is by multiplying the denominators together to make them equal.</t>
+  </si>
+  <si>
+    <t>Then multiply the numerators by the same amount from the denominator.</t>
+  </si>
+  <si>
+    <t>level_1_info_2_c</t>
+  </si>
+  <si>
+    <t>After that, you can add both fractions properly.</t>
+  </si>
+  <si>
+    <t>Now it’s your turn! Use the multiplier to make both denominators equal.</t>
+  </si>
+  <si>
+    <t>Go ahead and type in the correct answer by pressing on either slot!</t>
+  </si>
+  <si>
+    <t>Notice how both fractions now have the same unit sizes? They can now be added properly.</t>
   </si>
 </sst>
 </file>
@@ -189,9 +249,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,6 +713,86 @@
         <v>39</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
initial level 2 dialog/tutorial
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2A0586-DF60-433D-8119-5CAD8221B57D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B66F58-784D-4CF5-8DDB-1919D74D7894}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="1635" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Key</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t>Notice how both fractions now have the same unit sizes? They can now be added properly.</t>
+  </si>
+  <si>
+    <t>level_2_intro_1</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>card_drag_instruct</t>
+  </si>
+  <si>
+    <t>Drag a card to an empty slot.</t>
   </si>
 </sst>
 </file>
@@ -535,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,6 +805,22 @@
         <v>51</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
prep up level 5 stuff, texts and tutorial flow added.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E6E893-B43B-4B9F-8EFF-E65C57B21649}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BEA4EE-D1B7-4174-A9D1-F76319B9C85C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="1635" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="1650" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Key</t>
   </si>
@@ -218,6 +218,84 @@
   </si>
   <si>
     <t>Hit the seal with enough fractions to move it out of the way!</t>
+  </si>
+  <si>
+    <t>level_3_intro_1</t>
+  </si>
+  <si>
+    <t>level_3_intro_2</t>
+  </si>
+  <si>
+    <t>Watch out! A yeti is in the way!</t>
+  </si>
+  <si>
+    <t>We must withstand the freezing wind to proceed!</t>
+  </si>
+  <si>
+    <t>level_3_info_1</t>
+  </si>
+  <si>
+    <t>In order to succeed, you must subtract the fractional attack until it reaches below zero.</t>
+  </si>
+  <si>
+    <t>mixedNumber</t>
+  </si>
+  <si>
+    <t>Mixed Number</t>
+  </si>
+  <si>
+    <t>improperFraction</t>
+  </si>
+  <si>
+    <t>Improper Fraction</t>
+  </si>
+  <si>
+    <t>level_5_intro_1</t>
+  </si>
+  <si>
+    <t>After an onerous battle, Pengu must catch a breath of fresh air.</t>
+  </si>
+  <si>
+    <t>level_5_intro_2</t>
+  </si>
+  <si>
+    <t>level_5_info_1_a</t>
+  </si>
+  <si>
+    <t>As you can see, there is a mixed number in this operation.</t>
+  </si>
+  <si>
+    <t>level_5_info_1_b</t>
+  </si>
+  <si>
+    <t>A mixed number is made up of a whole number, and a fraction.</t>
+  </si>
+  <si>
+    <t>level_5_info_2_a</t>
+  </si>
+  <si>
+    <t>level_5_info_3_a</t>
+  </si>
+  <si>
+    <t>level_5_info_2_b</t>
+  </si>
+  <si>
+    <t>To convert a mixed number to an improper fraction: multiply the whole number with the denominator of the fraction.</t>
+  </si>
+  <si>
+    <t>Afterwards, add the result to the numerator.</t>
+  </si>
+  <si>
+    <t>level_5_info_3_b</t>
+  </si>
+  <si>
+    <t>Use this technique to help you out with tricky operations!</t>
+  </si>
+  <si>
+    <t>Help Pengu swim towards the land by adding up the distances using fractions!</t>
+  </si>
+  <si>
+    <t>You can drag the whole number towards the fraction, or vice-versa, to convert.</t>
   </si>
 </sst>
 </file>
@@ -553,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,6 +913,110 @@
         <v>65</v>
       </c>
     </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
level 5 and 7 anims, dialogs
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BEA4EE-D1B7-4174-A9D1-F76319B9C85C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0EDB22-F782-42D3-8E99-02B442EFF9F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="1650" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Key</t>
   </si>
@@ -292,10 +292,22 @@
     <t>Use this technique to help you out with tricky operations!</t>
   </si>
   <si>
-    <t>Help Pengu swim towards the land by adding up the distances using fractions!</t>
-  </si>
-  <si>
     <t>You can drag the whole number towards the fraction, or vice-versa, to convert.</t>
+  </si>
+  <si>
+    <t>Help Pengu swim towards the land!</t>
+  </si>
+  <si>
+    <t>level_7_intro_1</t>
+  </si>
+  <si>
+    <t>A boulder is blocking Pengu's path!</t>
+  </si>
+  <si>
+    <t>level_7_intro_2</t>
+  </si>
+  <si>
+    <t>It is time to unleash the most potent of Pengu's fractional powers!</t>
   </si>
 </sst>
 </file>
@@ -631,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +978,7 @@
         <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1006,7 +1018,7 @@
         <v>84</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1015,6 +1027,22 @@
       </c>
       <c r="B45" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
end stuff, remove "level progress" scene
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BFF434-51BC-4E9B-90A5-B51CED020BA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444F669B-2734-4FAA-9683-6B74794DDC1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="1650" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>Key</t>
   </si>
@@ -326,6 +326,30 @@
   </si>
   <si>
     <t>Written by: David Dionisio\nMusic from: Kevin Macleod</t>
+  </si>
+  <si>
+    <t>game_complete</t>
+  </si>
+  <si>
+    <t>game_complete_desc</t>
+  </si>
+  <si>
+    <t>Thank you for playing!</t>
+  </si>
+  <si>
+    <t>finish</t>
+  </si>
+  <si>
+    <t>FINISH</t>
+  </si>
+  <si>
+    <t>total_score</t>
+  </si>
+  <si>
+    <t>TOTAL SCORE:</t>
+  </si>
+  <si>
+    <t>Congratulations! You have uncovered the treasure!</t>
   </si>
 </sst>
 </file>
@@ -661,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1095,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -1079,12 +1103,50 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>93</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgraded to unity 2019.4.4, latest playmaker
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444F669B-2734-4FAA-9683-6B74794DDC1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5869CBEB-A55F-4C2B-B30D-266C99B9D085}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1650" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9405" yWindow="1815" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>level_1_intro_1</t>
   </si>
   <si>
-    <t>A chasm impedes Pengu's journey.</t>
-  </si>
-  <si>
     <t>level_1_intro_2</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
     <t>To convert a mixed number to an improper fraction: multiply the whole number with the denominator of the fraction.</t>
   </si>
   <si>
-    <t>Afterwards, add the result to the numerator.</t>
-  </si>
-  <si>
     <t>level_5_info_3_b</t>
   </si>
   <si>
@@ -350,6 +344,12 @@
   </si>
   <si>
     <t>Congratulations! You have uncovered the treasure!</t>
+  </si>
+  <si>
+    <t>After that, add the result to the numerator.</t>
+  </si>
+  <si>
+    <t>A cliff impedes Pengu's journey.</t>
   </si>
 </sst>
 </file>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,31 +740,31 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,231 +892,231 @@
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
         <v>48</v>
-      </c>
-      <c r="B32" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
         <v>59</v>
-      </c>
-      <c r="B33" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" t="s">
         <v>69</v>
-      </c>
-      <c r="B38" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
         <v>71</v>
-      </c>
-      <c r="B39" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
         <v>73</v>
-      </c>
-      <c r="B40" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" t="s">
         <v>80</v>
-      </c>
-      <c r="B44" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C51">
         <v>4</v>
@@ -1124,10 +1124,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -1135,18 +1135,18 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated language spreadsheet with spanish
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5869CBEB-A55F-4C2B-B30D-266C99B9D085}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2214A62E-43F0-477F-AEC5-71A98CA0DFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9405" yWindow="1815" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="2865" windowWidth="22875" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
+    <sheet name="es" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="161">
   <si>
     <t>Key</t>
   </si>
@@ -350,6 +351,159 @@
   </si>
   <si>
     <t>A cliff impedes Pengu's journey.</t>
+  </si>
+  <si>
+    <t>¡Bienvenido!</t>
+  </si>
+  <si>
+    <t>Prueba 123 123</t>
+  </si>
+  <si>
+    <t>Pengu\n&lt;size=30&gt;y el&lt;/size&gt;\nEncuentros improbables</t>
+  </si>
+  <si>
+    <t>JUGAR</t>
+  </si>
+  <si>
+    <t>CRÉDITOS</t>
+  </si>
+  <si>
+    <t>Escrito por: David Dionisio\r\nMúsica de: Kevin Macleod</t>
+  </si>
+  <si>
+    <t>OPCIONES</t>
+  </si>
+  <si>
+    <t>SONIDO</t>
+  </si>
+  <si>
+    <t>MÚSICA</t>
+  </si>
+  <si>
+    <t>DISCURSO</t>
+  </si>
+  <si>
+    <t>APAGADO</t>
+  </si>
+  <si>
+    <t>PRENDIDO</t>
+  </si>
+  <si>
+    <t>CERCA</t>
+  </si>
+  <si>
+    <t>ENVIAR</t>
+  </si>
+  <si>
+    <t>VICTORIA</t>
+  </si>
+  <si>
+    <t>ATAQUE</t>
+  </si>
+  <si>
+    <t>DEFENDER</t>
+  </si>
+  <si>
+    <t>RONDAS</t>
+  </si>
+  <si>
+    <t>COMPLETAR</t>
+  </si>
+  <si>
+    <t>REVIVIR PENALIZACIÓN</t>
+  </si>
+  <si>
+    <t>Un abismo impide el viaje de Pengu.</t>
+  </si>
+  <si>
+    <t>¡Ayuda a Pengu a salir determinando la distancia de la brecha usando fracciones!</t>
+  </si>
+  <si>
+    <t>Para sumar estas dos fracciones, debes hacer iguales los denominadores.</t>
+  </si>
+  <si>
+    <t>Una forma de hacerlo es multiplicando los denominadores juntos para hacerlos iguales.</t>
+  </si>
+  <si>
+    <t>Después de eso, puedes agregar ambas fracciones correctamente.</t>
+  </si>
+  <si>
+    <t>¡Ahora te toca a ti! Utilice el multiplicador para hacer que ambos denominadores sean iguales.</t>
+  </si>
+  <si>
+    <t>¿Observa cómo ambas fracciones tienen ahora los mismos tamaños de unidad? Ahora se pueden añadir correctamente.</t>
+  </si>
+  <si>
+    <t>Sigue adelante y escribe la respuesta correcta pulsando en cualquiera de las ranuras.</t>
+  </si>
+  <si>
+    <t>¡ÉXITO!</t>
+  </si>
+  <si>
+    <t>Arrastra una tarjeta a una ranura vacía.</t>
+  </si>
+  <si>
+    <t>Una vez más, un obstáculo bloquea el camino de Pengu. Esta vez, una foca elefante.</t>
+  </si>
+  <si>
+    <t>¡Golpea el sello con suficientes fracciones para sacarlo del camino!</t>
+  </si>
+  <si>
+    <t>¡Cuidado! ¡Un yeti se interviene en camino!</t>
+  </si>
+  <si>
+    <t>¡Debemos soportar el viento helado para continuar!</t>
+  </si>
+  <si>
+    <t>Para tener éxito, debes restar el ataque fraccional hasta que llegue por debajo de cero.</t>
+  </si>
+  <si>
+    <t>Número Mixto</t>
+  </si>
+  <si>
+    <t>Fracción Incorrecta</t>
+  </si>
+  <si>
+    <t>Después de una onerosa batalla, Pengu debe respirar aire fresco.</t>
+  </si>
+  <si>
+    <t>¡Ayuda a Pengu a nadar hacia la tierra!</t>
+  </si>
+  <si>
+    <t>Como puede ver, hay un número mixto en esta operación.</t>
+  </si>
+  <si>
+    <t>Un número mixto se compone de un número entero y una fracción.</t>
+  </si>
+  <si>
+    <t>Para convertir un número mixto en una fracción incorrecta: multiplique el número entero por el denominador de la fracción.</t>
+  </si>
+  <si>
+    <t>Después, suma el resultado al numerador.</t>
+  </si>
+  <si>
+    <t>Puede arrastrar el número entero hacia la fracción, o viceversa, para convertirlo.</t>
+  </si>
+  <si>
+    <t>¡Utiliza esta técnica para ayudarte con operaciones complicadas!</t>
+  </si>
+  <si>
+    <t>¡Una roca está bloqueando el camino de Pengu!</t>
+  </si>
+  <si>
+    <t>¡Es hora de desatar los poderes fraccionarios más potentes de Pengu!</t>
+  </si>
+  <si>
+    <t>¡En hora buena! ¡Has descubierto el tesoro!</t>
+  </si>
+  <si>
+    <t>¡Gracias por jugar!</t>
+  </si>
+  <si>
+    <t>ACABADO</t>
+  </si>
+  <si>
+    <t>PUNTOS TOTALES:</t>
   </si>
 </sst>
 </file>
@@ -687,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,4 +1307,472 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378259CE-7254-4D41-8071-513E48CCE9C3}">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="89" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added "continue" and "new"
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2214A62E-43F0-477F-AEC5-71A98CA0DFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC03383-E9E6-40B4-933B-7C0A5E7AC1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2865" windowWidth="22875" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="2865" windowWidth="22875" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="167">
   <si>
     <t>Key</t>
   </si>
@@ -504,6 +504,24 @@
   </si>
   <si>
     <t>PUNTOS TOTALES:</t>
+  </si>
+  <si>
+    <t>new_game</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>CONTINUAR</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>NUEVO JUEGO</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
   </si>
 </sst>
 </file>
@@ -839,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,6 +1321,22 @@
         <v>106</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1311,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378259CE-7254-4D41-8071-513E48CCE9C3}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,6 +1806,22 @@
         <v>160</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed spanish text fit and future languages (hopefully) for UI
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC03383-E9E6-40B4-933B-7C0A5E7AC1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C1220C-68EC-44F7-8800-AEF3852FCE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2865" windowWidth="22875" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="2865" windowWidth="31845" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -359,9 +359,6 @@
     <t>Prueba 123 123</t>
   </si>
   <si>
-    <t>Pengu\n&lt;size=30&gt;y el&lt;/size&gt;\nEncuentros improbables</t>
-  </si>
-  <si>
     <t>JUGAR</t>
   </si>
   <si>
@@ -522,6 +519,9 @@
   </si>
   <si>
     <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>Pengu\n&lt;size=30&gt;y el&lt;/size&gt;\nEncuentros Improbables</t>
   </si>
 </sst>
 </file>
@@ -859,7 +859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
@@ -1323,18 +1323,18 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1347,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378259CE-7254-4D41-8071-513E48CCE9C3}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,7 +1400,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
         <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1496,7 +1496,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
         <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,7 +1536,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1560,7 @@
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
         <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1605,7 +1605,7 @@
         <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
         <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1621,7 +1621,7 @@
         <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1629,7 +1629,7 @@
         <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1637,7 +1637,7 @@
         <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1645,7 +1645,7 @@
         <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1653,7 +1653,7 @@
         <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1661,7 +1661,7 @@
         <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1669,7 +1669,7 @@
         <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
         <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1685,7 +1685,7 @@
         <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
         <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1701,7 +1701,7 @@
         <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
         <v>77</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1717,7 +1717,7 @@
         <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1725,7 +1725,7 @@
         <v>81</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1733,7 +1733,7 @@
         <v>83</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1741,7 +1741,7 @@
         <v>82</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1757,7 +1757,7 @@
         <v>89</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>91</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1773,7 +1773,7 @@
         <v>100</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C51">
         <v>4</v>
@@ -1784,7 +1784,7 @@
         <v>101</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -1795,7 +1795,7 @@
         <v>103</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1803,23 +1803,23 @@
         <v>105</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>161</v>
+      </c>
+      <c r="B56" t="s">
         <v>162</v>
-      </c>
-      <c r="B56" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>